<commit_message>
valuation of panchakanya mandir added
</commit_message>
<xml_diff>
--- a/ofc/estimates/sana gaun dhal byabasthapan/sanagaun dhal byabasthapan.xlsx
+++ b/ofc/estimates/sana gaun dhal byabasthapan/sanagaun dhal byabasthapan.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\081_082\ofc\ofc\estimates\sana gaun dhal byabasthapan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\081-082\ofc\estimates\sana gaun dhal byabasthapan\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="WCR" sheetId="6" r:id="rId1"/>
@@ -42,7 +42,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'Estimate (3)'!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">WCR!$1:$12</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -230,16 +230,16 @@
     <t xml:space="preserve">Project:- सानागाउँ ढल व्यबस्थापन </t>
   </si>
   <si>
-    <t>Date:2081/09/28</t>
+    <t xml:space="preserve">Date:                  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
@@ -398,7 +398,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -408,7 +408,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -428,14 +428,14 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -444,7 +444,7 @@
     <xf numFmtId="1" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -469,7 +469,7 @@
     <xf numFmtId="1" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -502,7 +502,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -511,7 +511,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -526,7 +526,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -542,12 +542,30 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -573,22 +591,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -600,18 +612,6 @@
     </xf>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1235,106 +1235,106 @@
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="76" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-    </row>
-    <row r="2" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A2" s="77" t="s">
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+    </row>
+    <row r="2" spans="1:11" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
-      <c r="J2" s="77"/>
-      <c r="K2" s="77"/>
-    </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="78" t="s">
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="78"/>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="78"/>
-      <c r="K3" s="78"/>
-    </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="78" t="s">
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="70"/>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
-      <c r="J4" s="78"/>
-      <c r="K4" s="78"/>
-    </row>
-    <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="79" t="s">
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="70"/>
+      <c r="K4" s="70"/>
+    </row>
+    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="79"/>
-      <c r="C5" s="79"/>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="79"/>
-      <c r="G5" s="79"/>
-      <c r="H5" s="79"/>
-      <c r="I5" s="79"/>
-      <c r="J5" s="79"/>
-      <c r="K5" s="79"/>
-    </row>
-    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="71"/>
+      <c r="I5" s="71"/>
+      <c r="J5" s="71"/>
+      <c r="K5" s="71"/>
+    </row>
+    <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="74" t="e">
+      <c r="C6" s="66" t="e">
         <f>F18</f>
         <v>#REF!</v>
       </c>
-      <c r="D6" s="75"/>
+      <c r="D6" s="67"/>
       <c r="E6" s="9"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -1342,90 +1342,90 @@
         <v>20</v>
       </c>
       <c r="I6" s="8"/>
-      <c r="J6" s="74" t="e">
+      <c r="J6" s="66" t="e">
         <f>I18</f>
         <v>#REF!</v>
       </c>
-      <c r="K6" s="75"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K6" s="67"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69"/>
-      <c r="I7" s="70" t="s">
+      <c r="F7" s="75"/>
+      <c r="G7" s="75"/>
+      <c r="I7" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="70"/>
-      <c r="K7" s="70"/>
-    </row>
-    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="68" t="e">
+      <c r="J7" s="76"/>
+      <c r="K7" s="76"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="74" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
-      <c r="F8" s="68"/>
-      <c r="I8" s="71" t="s">
+      <c r="B8" s="74"/>
+      <c r="C8" s="74"/>
+      <c r="D8" s="74"/>
+      <c r="E8" s="74"/>
+      <c r="F8" s="74"/>
+      <c r="I8" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="71"/>
-      <c r="K8" s="71"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="72" t="e">
+      <c r="J8" s="77"/>
+      <c r="K8" s="77"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="78" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B9" s="72"/>
-      <c r="C9" s="72"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="72"/>
-      <c r="I9" s="71" t="s">
+      <c r="B9" s="78"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="78"/>
+      <c r="F9" s="78"/>
+      <c r="I9" s="77" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="71"/>
-      <c r="K9" s="71"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="66" t="s">
+      <c r="J9" s="77"/>
+      <c r="K9" s="77"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="66" t="s">
+      <c r="B11" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="66" t="s">
+      <c r="C11" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="73" t="s">
+      <c r="D11" s="79" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="73"/>
-      <c r="F11" s="73"/>
-      <c r="G11" s="73" t="s">
+      <c r="E11" s="79"/>
+      <c r="F11" s="79"/>
+      <c r="G11" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="73"/>
-      <c r="I11" s="73"/>
-      <c r="J11" s="66" t="s">
+      <c r="H11" s="79"/>
+      <c r="I11" s="79"/>
+      <c r="J11" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="67" t="s">
+      <c r="K11" s="73" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="66"/>
-      <c r="B12" s="66"/>
-      <c r="C12" s="66"/>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="72"/>
+      <c r="B12" s="72"/>
+      <c r="C12" s="72"/>
       <c r="D12" s="11" t="s">
         <v>26</v>
       </c>
@@ -1444,10 +1444,10 @@
       <c r="I12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="66"/>
-      <c r="K12" s="67"/>
-    </row>
-    <row r="13" spans="1:11" s="1" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="J12" s="72"/>
+      <c r="K12" s="73"/>
+    </row>
+    <row r="13" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -1490,7 +1490,7 @@
       </c>
       <c r="K13" s="14"/>
     </row>
-    <row r="14" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="27"/>
       <c r="B14" s="33" t="e">
         <f>#REF!</f>
@@ -1512,7 +1512,7 @@
       <c r="J14" s="28"/>
       <c r="K14" s="14"/>
     </row>
-    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="29"/>
       <c r="B15" s="29"/>
       <c r="C15" s="12"/>
@@ -1525,7 +1525,7 @@
       <c r="J15" s="28"/>
       <c r="K15" s="14"/>
     </row>
-    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -1568,7 +1568,7 @@
       </c>
       <c r="K16" s="14"/>
     </row>
-    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="29"/>
       <c r="B17" s="29"/>
       <c r="C17" s="12"/>
@@ -1581,7 +1581,7 @@
       <c r="J17" s="28"/>
       <c r="K17" s="14"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="6" t="s">
         <v>16</v>
@@ -1607,13 +1607,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A8:F8"/>
@@ -1627,6 +1620,13 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:I11"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1644,137 +1644,137 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="3" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.88671875" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="85" t="s">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
-      <c r="I1" s="85"/>
-      <c r="J1" s="85"/>
-      <c r="K1" s="85"/>
-    </row>
-    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="86" t="s">
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
+    </row>
+    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-    </row>
-    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="78" t="s">
+      <c r="B2" s="82"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="82"/>
+      <c r="K2" s="82"/>
+    </row>
+    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="78"/>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="78"/>
-      <c r="K3" s="78"/>
-    </row>
-    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="78" t="s">
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="70"/>
+    </row>
+    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
-      <c r="J4" s="78"/>
-      <c r="K4" s="78"/>
-    </row>
-    <row r="5" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="87" t="s">
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="70"/>
+      <c r="K4" s="70"/>
+    </row>
+    <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="87"/>
-      <c r="C5" s="87"/>
-      <c r="D5" s="87"/>
-      <c r="E5" s="87"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="87"/>
-      <c r="H5" s="87"/>
-      <c r="I5" s="87"/>
-      <c r="J5" s="87"/>
-      <c r="K5" s="87"/>
-    </row>
-    <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="68" t="s">
+      <c r="B5" s="83"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="83"/>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="74" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="68"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
+      <c r="B6" s="74"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="74"/>
+      <c r="E6" s="74"/>
+      <c r="F6" s="74"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="84" t="s">
+      <c r="H6" s="80" t="s">
         <v>46</v>
       </c>
-      <c r="I6" s="84"/>
-      <c r="J6" s="84"/>
-      <c r="K6" s="84"/>
+      <c r="I6" s="80"/>
+      <c r="J6" s="80"/>
+      <c r="K6" s="80"/>
       <c r="O6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="81" t="s">
+    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="81"/>
-      <c r="C7" s="81"/>
-      <c r="D7" s="81"/>
-      <c r="E7" s="81"/>
-      <c r="F7" s="81"/>
+      <c r="B7" s="85"/>
+      <c r="C7" s="85"/>
+      <c r="D7" s="85"/>
+      <c r="E7" s="85"/>
+      <c r="F7" s="85"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="82" t="s">
+      <c r="H7" s="86" t="s">
         <v>56</v>
       </c>
-      <c r="I7" s="82"/>
-      <c r="J7" s="82"/>
-      <c r="K7" s="82"/>
-    </row>
-    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I7" s="86"/>
+      <c r="J7" s="86"/>
+      <c r="K7" s="86"/>
+    </row>
+    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -1812,7 +1812,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="138" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" ht="150" x14ac:dyDescent="0.25">
       <c r="A9" s="29">
         <v>1</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
       <c r="B10" s="38" t="s">
         <v>50</v>
@@ -1871,7 +1871,7 @@
       <c r="R10" s="25"/>
       <c r="S10" s="25"/>
     </row>
-    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="B11" s="38" t="s">
         <v>42</v>
@@ -1903,7 +1903,7 @@
       <c r="R11" s="25"/>
       <c r="S11" s="25"/>
     </row>
-    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="B12" s="38" t="s">
         <v>40</v>
@@ -1928,7 +1928,7 @@
       <c r="R12" s="25"/>
       <c r="S12" s="25"/>
     </row>
-    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18"/>
       <c r="B13" s="38"/>
       <c r="C13" s="19"/>
@@ -1948,7 +1948,7 @@
       <c r="R13" s="25"/>
       <c r="S13" s="25"/>
     </row>
-    <row r="14" spans="1:19" ht="96.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="18">
         <v>2</v>
       </c>
@@ -1972,7 +1972,7 @@
       <c r="R14" s="25"/>
       <c r="S14" s="25"/>
     </row>
-    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
       <c r="B15" s="38" t="s">
         <v>43</v>
@@ -2006,7 +2006,7 @@
       <c r="R15" s="25"/>
       <c r="S15" s="25"/>
     </row>
-    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
       <c r="B16" s="38" t="s">
         <v>42</v>
@@ -2038,7 +2038,7 @@
       <c r="R16" s="25"/>
       <c r="S16" s="25"/>
     </row>
-    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
       <c r="B17" s="38"/>
       <c r="C17" s="19"/>
@@ -2058,7 +2058,7 @@
       <c r="R17" s="25"/>
       <c r="S17" s="25"/>
     </row>
-    <row r="18" spans="1:19" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="18">
         <v>3</v>
       </c>
@@ -2082,7 +2082,7 @@
       <c r="R18" s="25"/>
       <c r="S18" s="25"/>
     </row>
-    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
       <c r="B19" s="38" t="s">
         <v>43</v>
@@ -2117,7 +2117,7 @@
       <c r="R19" s="25"/>
       <c r="S19" s="25"/>
     </row>
-    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="41"/>
       <c r="B20" s="38" t="s">
         <v>42</v>
@@ -2142,7 +2142,7 @@
       </c>
       <c r="K20" s="37"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="41"/>
       <c r="B21" s="38" t="s">
         <v>40</v>
@@ -2160,7 +2160,7 @@
       </c>
       <c r="K21" s="37"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="41"/>
       <c r="B22" s="38"/>
       <c r="C22" s="43"/>
@@ -2173,7 +2173,7 @@
       <c r="J22" s="46"/>
       <c r="K22" s="37"/>
     </row>
-    <row r="23" spans="1:19" ht="69" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="18">
         <v>4</v>
       </c>
@@ -2197,7 +2197,7 @@
       <c r="R23" s="25"/>
       <c r="S23" s="25"/>
     </row>
-    <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18"/>
       <c r="B24" s="38" t="s">
         <v>50</v>
@@ -2232,7 +2232,7 @@
       <c r="R24" s="25"/>
       <c r="S24" s="25"/>
     </row>
-    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="18"/>
       <c r="B25" s="38"/>
       <c r="C25" s="37">
@@ -2264,7 +2264,7 @@
       <c r="R25" s="25"/>
       <c r="S25" s="25"/>
     </row>
-    <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="41"/>
       <c r="B26" s="38" t="s">
         <v>42</v>
@@ -2289,7 +2289,7 @@
       </c>
       <c r="K26" s="37"/>
     </row>
-    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="41"/>
       <c r="B27" s="38" t="s">
         <v>40</v>
@@ -2307,7 +2307,7 @@
       </c>
       <c r="K27" s="37"/>
     </row>
-    <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="41"/>
       <c r="B28" s="38"/>
       <c r="C28" s="43"/>
@@ -2320,7 +2320,7 @@
       <c r="J28" s="46"/>
       <c r="K28" s="37"/>
     </row>
-    <row r="29" spans="1:19" s="1" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" s="64">
         <v>5</v>
       </c>
@@ -2337,7 +2337,7 @@
       <c r="J29" s="46"/>
       <c r="K29" s="29"/>
     </row>
-    <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="18"/>
       <c r="B30" s="38" t="s">
         <v>50</v>
@@ -2371,7 +2371,7 @@
       <c r="R30" s="25"/>
       <c r="S30" s="25"/>
     </row>
-    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="41"/>
       <c r="B31" s="38" t="s">
         <v>42</v>
@@ -2396,7 +2396,7 @@
       </c>
       <c r="K31" s="37"/>
     </row>
-    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="41"/>
       <c r="B32" s="38" t="s">
         <v>40</v>
@@ -2414,7 +2414,7 @@
       </c>
       <c r="K32" s="37"/>
     </row>
-    <row r="33" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="41"/>
       <c r="B33" s="38"/>
       <c r="C33" s="43"/>
@@ -2427,7 +2427,7 @@
       <c r="J33" s="45"/>
       <c r="K33" s="37"/>
     </row>
-    <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="18">
         <v>6</v>
       </c>
@@ -2463,7 +2463,7 @@
       <c r="R34" s="25"/>
       <c r="S34" s="25"/>
     </row>
-    <row r="35" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="18"/>
       <c r="B35" s="24"/>
       <c r="C35" s="19"/>
@@ -2486,7 +2486,7 @@
       <c r="R35" s="25"/>
       <c r="S35" s="25"/>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="41"/>
       <c r="B36" s="47" t="s">
         <v>17</v>
@@ -2504,7 +2504,7 @@
       </c>
       <c r="K36" s="37"/>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="59"/>
       <c r="B37" s="62"/>
       <c r="C37" s="63"/>
@@ -2517,16 +2517,16 @@
       <c r="J37" s="61"/>
       <c r="K37" s="58"/>
     </row>
-    <row r="38" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="51"/>
       <c r="B38" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C38" s="80">
+      <c r="C38" s="84">
         <f>J36</f>
         <v>447610.12228750001</v>
       </c>
-      <c r="D38" s="80"/>
+      <c r="D38" s="84"/>
       <c r="E38" s="40">
         <v>100</v>
       </c>
@@ -2537,15 +2537,15 @@
       <c r="J38" s="55"/>
       <c r="K38" s="56"/>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="57"/>
       <c r="B39" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C39" s="83">
+      <c r="C39" s="87">
         <v>400000</v>
       </c>
-      <c r="D39" s="83"/>
+      <c r="D39" s="87"/>
       <c r="E39" s="40"/>
       <c r="F39" s="50"/>
       <c r="G39" s="49"/>
@@ -2554,16 +2554,16 @@
       <c r="J39" s="49"/>
       <c r="K39" s="50"/>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="57"/>
       <c r="B40" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C40" s="83">
+      <c r="C40" s="87">
         <f>C39-C42-C43</f>
         <v>380000</v>
       </c>
-      <c r="D40" s="83"/>
+      <c r="D40" s="87"/>
       <c r="E40" s="40">
         <f>C40/C38*100</f>
         <v>84.895309797289613</v>
@@ -2575,16 +2575,16 @@
       <c r="J40" s="49"/>
       <c r="K40" s="50"/>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="57"/>
       <c r="B41" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C41" s="80">
+      <c r="C41" s="84">
         <f>C38-C40</f>
         <v>67610.122287500009</v>
       </c>
-      <c r="D41" s="80"/>
+      <c r="D41" s="84"/>
       <c r="E41" s="40">
         <f>100-E40</f>
         <v>15.104690202710387</v>
@@ -2596,16 +2596,16 @@
       <c r="J41" s="49"/>
       <c r="K41" s="50"/>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="57"/>
       <c r="B42" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C42" s="80">
+      <c r="C42" s="84">
         <f>C39*0.03</f>
         <v>12000</v>
       </c>
-      <c r="D42" s="80"/>
+      <c r="D42" s="84"/>
       <c r="E42" s="40">
         <v>3</v>
       </c>
@@ -2616,16 +2616,16 @@
       <c r="J42" s="49"/>
       <c r="K42" s="50"/>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="57"/>
       <c r="B43" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C43" s="80">
+      <c r="C43" s="84">
         <f>C39*0.02</f>
         <v>8000</v>
       </c>
-      <c r="D43" s="80"/>
+      <c r="D43" s="84"/>
       <c r="E43" s="40">
         <v>2</v>
       </c>
@@ -2636,7 +2636,7 @@
       <c r="J43" s="49"/>
       <c r="K43" s="50"/>
     </row>
-    <row r="44" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="58"/>
       <c r="B44" s="58"/>
       <c r="C44" s="58"/>
@@ -2649,71 +2649,64 @@
       <c r="J44" s="58"/>
       <c r="K44" s="58"/>
     </row>
-    <row r="45" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="49" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="50" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="51" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="52" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="53" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="54" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="55" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="56" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="57" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="58" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="59" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="60" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="61" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="62" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="63" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="64" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="65" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="66" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="67" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="68" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="69" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="70" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="71" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="72" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="73" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="74" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="75" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="76" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="77" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="78" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="79" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="80" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="81" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="82" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="83" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="84" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="85" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="86" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="87" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="88" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="89" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="90" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="91" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="92" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="93" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="94" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="95" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="96" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="97" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="98" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="99" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="100" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="86" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="88" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="89" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="90" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="94" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="95" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="96" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="97" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="98" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="99" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="100" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C42:D42"/>
     <mergeCell ref="C43:D43"/>
     <mergeCell ref="A7:F7"/>
@@ -2722,6 +2715,13 @@
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="C40:D40"/>
     <mergeCell ref="C41:D41"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>

</xml_diff>